<commit_message>
Running program for video
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/526ee003691b220b/Documents/University/Year_4/4OI6/Project/.venv/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/526ee003691b220b/Documents/University/Year_4/4OI6/CapstoneProject/Capstone/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="8_{7F8EF400-FA14-4360-BE3A-91428D8CCAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{50F69750-FF17-4C92-B7B1-0E4F1011DF1C}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="8_{7F8EF400-FA14-4360-BE3A-91428D8CCAE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9A483C5A-21E2-4144-80FB-1BC13929B898}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{CB6CCB61-2F99-4CA9-8831-150E9C59DA18}"/>
   </bookViews>
@@ -83,10 +83,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -409,7 +405,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -417,11 +413,11 @@
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>86.37</v>
+        <v>81.06</v>
       </c>
       <c r="B1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>40.770000000000003</v>
+        <v>94.84</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -431,53 +427,53 @@
       </c>
       <c r="E1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>48.72</v>
+        <v>48.79</v>
       </c>
       <c r="F1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>29.25</v>
+        <v>43.23</v>
       </c>
       <c r="G1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>20.45</v>
+        <v>86.08</v>
       </c>
       <c r="H1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>90.48</v>
+        <v>68.180000000000007</v>
       </c>
       <c r="I1">
         <f ca="1">INT(RAND()*100)</f>
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="J1">
         <f ca="1">INT(RAND()*100)</f>
-        <v>45</v>
+        <v>93</v>
       </c>
       <c r="K1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>25.96</v>
+        <v>36.590000000000003</v>
       </c>
       <c r="L1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>40.340000000000003</v>
+        <v>47.96</v>
       </c>
       <c r="M1">
         <f ca="1">INT(RAND()*100)</f>
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="N1">
         <f ca="1">INT(RAND()*100)</f>
-        <v>18</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <f t="shared" ref="A2:B3" ca="1" si="0">ROUND(RAND()*100,2)</f>
-        <v>22.88</v>
+        <v>3.35</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>61.53</v>
+        <v>46.34</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -492,50 +488,50 @@
         <v>20</v>
       </c>
       <c r="G2">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="H2">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I2">
         <v>0</v>
       </c>
       <c r="J2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="K2">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="L2">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="M2">
         <v>0</v>
       </c>
       <c r="N2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="O2">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="P2">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="Q2">
         <v>0</v>
       </c>
       <c r="R2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>91.29</v>
+        <v>44.97</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>94.54</v>
+        <v>33.22</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -545,53 +541,53 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:H3" ca="1" si="1">ROUND(RAND()*100,2)</f>
-        <v>19.77</v>
+        <v>61.07</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>40.31</v>
+        <v>21.49</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
-        <v>83.6</v>
+        <v>10.119999999999999</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>48.8</v>
+        <v>97.15</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:J3" ca="1" si="2">INT(RAND()*100)</f>
-        <v>47</v>
+        <v>74</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="2"/>
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:L3" ca="1" si="3">ROUND(RAND()*100,2)</f>
-        <v>71.94</v>
+        <v>36.64</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="3"/>
-        <v>86.04</v>
+        <v>74.8</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:N3" ca="1" si="4">INT(RAND()*100)</f>
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="N3">
         <f t="shared" ca="1" si="4"/>
-        <v>91</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" ref="A5:B10" ca="1" si="5">ROUND(RAND()*100,2)</f>
-        <v>15.78</v>
+        <v>61.41</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="5"/>
-        <v>69.38</v>
+        <v>27.04</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -621,11 +617,11 @@
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" ca="1" si="5"/>
-        <v>57.71</v>
+        <v>61.71</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="5"/>
-        <v>9.7100000000000009</v>
+        <v>0.05</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -634,54 +630,56 @@
         <v>0</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E5:H10" ca="1" si="6">ROUND(RAND()*100,2)</f>
-        <v>69.31</v>
+        <v>20</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="6"/>
-        <v>72.16</v>
+        <v>20</v>
       </c>
       <c r="G6">
-        <f t="shared" ca="1" si="6"/>
-        <v>86.03</v>
+        <v>22</v>
       </c>
       <c r="H6">
-        <f t="shared" ca="1" si="6"/>
-        <v>49.39</v>
+        <v>22</v>
       </c>
       <c r="I6">
-        <f t="shared" ref="I5:J10" ca="1" si="7">INT(RAND()*100)</f>
-        <v>54</v>
+        <v>0</v>
       </c>
       <c r="J6">
-        <f t="shared" ca="1" si="7"/>
-        <v>65</v>
+        <v>1</v>
       </c>
       <c r="K6">
-        <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>75.39</v>
+        <v>24</v>
       </c>
       <c r="L6">
-        <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>3.75</v>
+        <v>24</v>
       </c>
       <c r="M6">
-        <f ca="1">INT(RAND()*100)</f>
-        <v>49</v>
+        <v>0</v>
       </c>
       <c r="N6">
-        <f ca="1">INT(RAND()*100)</f>
-        <v>83</v>
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>26</v>
+      </c>
+      <c r="P6">
+        <v>26</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" ca="1" si="5"/>
-        <v>47.11</v>
+        <v>53.14</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="5"/>
-        <v>11.01</v>
+        <v>99.31</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -690,70 +688,70 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" ca="1" si="6"/>
-        <v>69.239999999999995</v>
+        <f t="shared" ref="E6:H10" ca="1" si="6">ROUND(RAND()*100,2)</f>
+        <v>63.83</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="6"/>
-        <v>8.69</v>
+        <v>82.6</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="6"/>
-        <v>77.44</v>
+        <v>76.36</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="6"/>
-        <v>93.37</v>
+        <v>70.69</v>
       </c>
       <c r="I7">
-        <f t="shared" ca="1" si="7"/>
-        <v>93</v>
+        <f t="shared" ref="I6:J10" ca="1" si="7">INT(RAND()*100)</f>
+        <v>19</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="7"/>
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="K7">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>93.45</v>
+        <v>88.5</v>
       </c>
       <c r="L7">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>78.349999999999994</v>
+        <v>25.6</v>
       </c>
       <c r="M7">
         <f ca="1">INT(RAND()*100)</f>
-        <v>31</v>
+        <v>8</v>
       </c>
       <c r="N7">
         <f ca="1">INT(RAND()*100)</f>
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="O7">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>4.46</v>
+        <v>36.68</v>
       </c>
       <c r="P7">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>82.46</v>
+        <v>68.98</v>
       </c>
       <c r="Q7">
         <f ca="1">INT(RAND()*100)</f>
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="R7">
         <f ca="1">INT(RAND()*100)</f>
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" ca="1" si="5"/>
-        <v>63.71</v>
+        <v>25.44</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="5"/>
-        <v>0.16</v>
+        <v>53.96</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -763,37 +761,37 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="6"/>
-        <v>34.68</v>
+        <v>97.54</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="6"/>
-        <v>63.61</v>
+        <v>50.08</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="6"/>
-        <v>71.38</v>
+        <v>29.72</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="6"/>
-        <v>50.93</v>
+        <v>51.27</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="7"/>
-        <v>76</v>
+        <v>3</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="7"/>
-        <v>63</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" ca="1" si="5"/>
-        <v>62.81</v>
+        <v>6.58</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="5"/>
-        <v>22.81</v>
+        <v>41.07</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -803,53 +801,53 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="6"/>
-        <v>47.21</v>
+        <v>89.59</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="6"/>
-        <v>84.38</v>
+        <v>15.91</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="6"/>
-        <v>33.01</v>
+        <v>21.48</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="6"/>
-        <v>68.81</v>
+        <v>10.38</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="7"/>
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="7"/>
-        <v>74</v>
+        <v>48</v>
       </c>
       <c r="K9">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>60.91</v>
+        <v>12.02</v>
       </c>
       <c r="L9">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>44.23</v>
+        <v>73.209999999999994</v>
       </c>
       <c r="M9">
         <f ca="1">INT(RAND()*100)</f>
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="N9">
         <f ca="1">INT(RAND()*100)</f>
-        <v>53</v>
+        <v>93</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" ca="1" si="5"/>
-        <v>34.79</v>
+        <v>41.06</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="5"/>
-        <v>88.88</v>
+        <v>37.659999999999997</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -859,59 +857,59 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="6"/>
-        <v>84.48</v>
+        <v>96.18</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="6"/>
-        <v>94.31</v>
+        <v>64.11</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="6"/>
-        <v>55.3</v>
+        <v>57.6</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="6"/>
-        <v>45.25</v>
+        <v>32.57</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="7"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="7"/>
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <f ca="1">ROUND(RAND()*100,2)</f>
+        <v>90.62</v>
+      </c>
+      <c r="L10">
+        <f ca="1">ROUND(RAND()*100,2)</f>
+        <v>22.25</v>
+      </c>
+      <c r="M10">
+        <f ca="1">INT(RAND()*100)</f>
         <v>19</v>
       </c>
-      <c r="K10">
-        <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>26.06</v>
-      </c>
-      <c r="L10">
-        <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>23.59</v>
-      </c>
-      <c r="M10">
-        <f ca="1">INT(RAND()*100)</f>
-        <v>85</v>
-      </c>
       <c r="N10">
         <f ca="1">INT(RAND()*100)</f>
-        <v>61</v>
+        <v>8</v>
       </c>
       <c r="O10">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>18.25</v>
+        <v>50.83</v>
       </c>
       <c r="P10">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>15.64</v>
+        <v>74.48</v>
       </c>
       <c r="Q10">
         <f ca="1">INT(RAND()*100)</f>
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="R10">
         <f ca="1">INT(RAND()*100)</f>
-        <v>23</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
No more while loop sin thermotron class, all moved to script
</commit_message>
<xml_diff>
--- a/programs.xlsx
+++ b/programs.xlsx
@@ -83,6 +83,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -405,7 +409,7 @@
   <dimension ref="A1:R10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -413,11 +417,11 @@
     <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>81.06</v>
+        <v>98.91</v>
       </c>
       <c r="B1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>94.84</v>
+        <v>13.72</v>
       </c>
       <c r="C1">
         <v>0</v>
@@ -427,53 +431,53 @@
       </c>
       <c r="E1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>48.79</v>
+        <v>96.46</v>
       </c>
       <c r="F1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>43.23</v>
+        <v>60.91</v>
       </c>
       <c r="G1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>86.08</v>
+        <v>78.489999999999995</v>
       </c>
       <c r="H1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>68.180000000000007</v>
+        <v>32.67</v>
       </c>
       <c r="I1">
         <f ca="1">INT(RAND()*100)</f>
-        <v>61</v>
+        <v>46</v>
       </c>
       <c r="J1">
         <f ca="1">INT(RAND()*100)</f>
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="K1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>36.590000000000003</v>
+        <v>26.13</v>
       </c>
       <c r="L1">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>47.96</v>
+        <v>24.53</v>
       </c>
       <c r="M1">
         <f ca="1">INT(RAND()*100)</f>
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="N1">
         <f ca="1">INT(RAND()*100)</f>
-        <v>25</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A2">
         <f t="shared" ref="A2:B3" ca="1" si="0">ROUND(RAND()*100,2)</f>
-        <v>3.35</v>
+        <v>9.07</v>
       </c>
       <c r="B2">
         <f t="shared" ca="1" si="0"/>
-        <v>46.34</v>
+        <v>59.89</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -527,11 +531,11 @@
     <row r="3" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A3">
         <f t="shared" ca="1" si="0"/>
-        <v>44.97</v>
+        <v>59.61</v>
       </c>
       <c r="B3">
         <f t="shared" ca="1" si="0"/>
-        <v>33.22</v>
+        <v>59.95</v>
       </c>
       <c r="C3">
         <v>0</v>
@@ -541,53 +545,53 @@
       </c>
       <c r="E3">
         <f t="shared" ref="E3:H3" ca="1" si="1">ROUND(RAND()*100,2)</f>
-        <v>61.07</v>
+        <v>78.709999999999994</v>
       </c>
       <c r="F3">
         <f t="shared" ca="1" si="1"/>
-        <v>21.49</v>
+        <v>26.08</v>
       </c>
       <c r="G3">
         <f t="shared" ca="1" si="1"/>
-        <v>10.119999999999999</v>
+        <v>53.35</v>
       </c>
       <c r="H3">
         <f t="shared" ca="1" si="1"/>
-        <v>97.15</v>
+        <v>65.430000000000007</v>
       </c>
       <c r="I3">
         <f t="shared" ref="I3:J3" ca="1" si="2">INT(RAND()*100)</f>
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="J3">
         <f t="shared" ca="1" si="2"/>
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:L3" ca="1" si="3">ROUND(RAND()*100,2)</f>
-        <v>36.64</v>
+        <v>40.17</v>
       </c>
       <c r="L3">
         <f t="shared" ca="1" si="3"/>
-        <v>74.8</v>
+        <v>30.15</v>
       </c>
       <c r="M3">
         <f t="shared" ref="M3:N3" ca="1" si="4">INT(RAND()*100)</f>
-        <v>85</v>
+        <v>50</v>
       </c>
       <c r="N3">
         <f t="shared" ca="1" si="4"/>
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" ref="A5:B10" ca="1" si="5">ROUND(RAND()*100,2)</f>
-        <v>61.41</v>
+        <v>33.94</v>
       </c>
       <c r="B5">
         <f t="shared" ca="1" si="5"/>
-        <v>27.04</v>
+        <v>17.77</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -617,11 +621,11 @@
     <row r="6" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" ca="1" si="5"/>
-        <v>61.71</v>
+        <v>62.05</v>
       </c>
       <c r="B6">
         <f t="shared" ca="1" si="5"/>
-        <v>0.05</v>
+        <v>5.68</v>
       </c>
       <c r="C6">
         <v>0</v>
@@ -675,11 +679,11 @@
     <row r="7" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" ca="1" si="5"/>
-        <v>53.14</v>
+        <v>92.46</v>
       </c>
       <c r="B7">
         <f t="shared" ca="1" si="5"/>
-        <v>99.31</v>
+        <v>83.61</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -688,70 +692,70 @@
         <v>0</v>
       </c>
       <c r="E7">
-        <f t="shared" ref="E6:H10" ca="1" si="6">ROUND(RAND()*100,2)</f>
-        <v>63.83</v>
+        <f t="shared" ref="E7:H10" ca="1" si="6">ROUND(RAND()*100,2)</f>
+        <v>49.65</v>
       </c>
       <c r="F7">
         <f t="shared" ca="1" si="6"/>
-        <v>82.6</v>
+        <v>42.78</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="6"/>
-        <v>76.36</v>
+        <v>22.34</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="6"/>
-        <v>70.69</v>
+        <v>18.04</v>
       </c>
       <c r="I7">
-        <f t="shared" ref="I6:J10" ca="1" si="7">INT(RAND()*100)</f>
-        <v>19</v>
+        <f t="shared" ref="I7:J10" ca="1" si="7">INT(RAND()*100)</f>
+        <v>96</v>
       </c>
       <c r="J7">
         <f t="shared" ca="1" si="7"/>
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="K7">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>88.5</v>
+        <v>74.25</v>
       </c>
       <c r="L7">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>25.6</v>
+        <v>58.88</v>
       </c>
       <c r="M7">
         <f ca="1">INT(RAND()*100)</f>
-        <v>8</v>
+        <v>55</v>
       </c>
       <c r="N7">
         <f ca="1">INT(RAND()*100)</f>
-        <v>77</v>
+        <v>15</v>
       </c>
       <c r="O7">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>36.68</v>
+        <v>83.26</v>
       </c>
       <c r="P7">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>68.98</v>
+        <v>77.599999999999994</v>
       </c>
       <c r="Q7">
         <f ca="1">INT(RAND()*100)</f>
-        <v>45</v>
+        <v>2</v>
       </c>
       <c r="R7">
         <f ca="1">INT(RAND()*100)</f>
-        <v>28</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" ca="1" si="5"/>
-        <v>25.44</v>
+        <v>52.02</v>
       </c>
       <c r="B8">
         <f t="shared" ca="1" si="5"/>
-        <v>53.96</v>
+        <v>20.53</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -761,37 +765,37 @@
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="6"/>
-        <v>97.54</v>
+        <v>38.24</v>
       </c>
       <c r="F8">
         <f t="shared" ca="1" si="6"/>
-        <v>50.08</v>
+        <v>61.43</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="6"/>
-        <v>29.72</v>
+        <v>2.31</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="6"/>
-        <v>51.27</v>
+        <v>19.28</v>
       </c>
       <c r="I8">
         <f t="shared" ca="1" si="7"/>
-        <v>3</v>
+        <v>93</v>
       </c>
       <c r="J8">
         <f t="shared" ca="1" si="7"/>
-        <v>1</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" ca="1" si="5"/>
-        <v>6.58</v>
+        <v>41.21</v>
       </c>
       <c r="B9">
         <f t="shared" ca="1" si="5"/>
-        <v>41.07</v>
+        <v>50.08</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -801,53 +805,53 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="6"/>
-        <v>89.59</v>
+        <v>45.63</v>
       </c>
       <c r="F9">
         <f t="shared" ca="1" si="6"/>
-        <v>15.91</v>
+        <v>56.27</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="6"/>
-        <v>21.48</v>
+        <v>1.94</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="6"/>
-        <v>10.38</v>
+        <v>37.950000000000003</v>
       </c>
       <c r="I9">
         <f t="shared" ca="1" si="7"/>
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="J9">
         <f t="shared" ca="1" si="7"/>
-        <v>48</v>
+        <v>23</v>
       </c>
       <c r="K9">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>12.02</v>
+        <v>15.29</v>
       </c>
       <c r="L9">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>73.209999999999994</v>
+        <v>32.72</v>
       </c>
       <c r="M9">
         <f ca="1">INT(RAND()*100)</f>
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="N9">
         <f ca="1">INT(RAND()*100)</f>
-        <v>93</v>
+        <v>40</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" ca="1" si="5"/>
-        <v>41.06</v>
+        <v>19.440000000000001</v>
       </c>
       <c r="B10">
         <f t="shared" ca="1" si="5"/>
-        <v>37.659999999999997</v>
+        <v>50.14</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -857,51 +861,51 @@
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="6"/>
-        <v>96.18</v>
+        <v>57.59</v>
       </c>
       <c r="F10">
         <f t="shared" ca="1" si="6"/>
-        <v>64.11</v>
+        <v>65.03</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="6"/>
-        <v>57.6</v>
+        <v>19.02</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="6"/>
-        <v>32.57</v>
+        <v>76.459999999999994</v>
       </c>
       <c r="I10">
         <f t="shared" ca="1" si="7"/>
-        <v>17</v>
+        <v>84</v>
       </c>
       <c r="J10">
         <f t="shared" ca="1" si="7"/>
-        <v>9</v>
+        <v>96</v>
       </c>
       <c r="K10">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>90.62</v>
+        <v>0.41</v>
       </c>
       <c r="L10">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>22.25</v>
+        <v>30.69</v>
       </c>
       <c r="M10">
         <f ca="1">INT(RAND()*100)</f>
-        <v>19</v>
+        <v>61</v>
       </c>
       <c r="N10">
         <f ca="1">INT(RAND()*100)</f>
-        <v>8</v>
+        <v>77</v>
       </c>
       <c r="O10">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>50.83</v>
+        <v>90.25</v>
       </c>
       <c r="P10">
         <f ca="1">ROUND(RAND()*100,2)</f>
-        <v>74.48</v>
+        <v>27.34</v>
       </c>
       <c r="Q10">
         <f ca="1">INT(RAND()*100)</f>
@@ -909,7 +913,7 @@
       </c>
       <c r="R10">
         <f ca="1">INT(RAND()*100)</f>
-        <v>76</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>